<commit_message>
Add stimuli structure files
</commit_message>
<xml_diff>
--- a/brainy-ideas/readAloud-valence-jess/data/pos-neg_dolphins_coding.xlsx
+++ b/brainy-ideas/readAloud-valence-jess/data/pos-neg_dolphins_coding.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/brainBox/brainy-ideas/rwe-valence-jess/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessraissouni/github/brainBox/brainy-ideas/readAloud-valence-jess/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD2A84-D899-3D4A-8B5B-7FFA72F4B725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071E303-6C2C-CF41-8456-60672FDEA7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="14820" xr2:uid="{64BEA42B-0FCC-E44A-8151-F26A63B588A7}"/>
+    <workbookView xWindow="0" yWindow="5420" windowWidth="27640" windowHeight="9900" xr2:uid="{64BEA42B-0FCC-E44A-8151-F26A63B588A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="259">
   <si>
     <t>in</t>
   </si>
@@ -105,9 +105,6 @@
     <t>per</t>
   </si>
   <si>
-    <t>depths</t>
-  </si>
-  <si>
     <t>and</t>
   </si>
   <si>
@@ -411,9 +408,6 @@
     <t>–cy,</t>
   </si>
   <si>
-    <t>–ters,</t>
-  </si>
-  <si>
     <t>dee</t>
   </si>
   <si>
@@ -510,9 +504,6 @@
     <t>–steemed</t>
   </si>
   <si>
-    <t>–e</t>
-  </si>
-  <si>
     <t>–pers</t>
   </si>
   <si>
@@ -805,6 +796,12 @@
   </si>
   <si>
     <t>duplicated syllable (0=no, 1=yes)</t>
+  </si>
+  <si>
+    <t>depths,</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1168,7 @@
   <dimension ref="A1:NB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="FQ1" sqref="FQ1:NB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,10 +1178,10 @@
   <sheetData>
     <row r="1" spans="1:366" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1193,28 +1190,28 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
@@ -1223,7 +1220,7 @@
         <v>7</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>8</v>
@@ -1232,34 +1229,34 @@
         <v>9</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>12</v>
@@ -1271,7 +1268,7 @@
         <v>14</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>15</v>
@@ -1280,22 +1277,22 @@
         <v>16</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AM1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>19</v>
@@ -1313,82 +1310,82 @@
         <v>22</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AX1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BG1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BJ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BL1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="BO1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="BT1" s="1" t="s">
         <v>1</v>
@@ -1397,190 +1394,190 @@
         <v>12</v>
       </c>
       <c r="BV1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="CC1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BX1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CE1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BZ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="CK1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="CG1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="CI1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CP1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="CQ1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="CV1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="CZ1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DC1" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="DD1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="DE1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="DF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DL1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="DN1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="DH1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="DR1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="DM1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="DS1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="DT1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="DW1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="DU1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="EA1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="DX1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="EB1" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="EC1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="ED1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="EE1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="EF1" s="1" t="s">
         <v>15</v>
@@ -1589,94 +1586,94 @@
         <v>12</v>
       </c>
       <c r="EH1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="EI1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="EI1" s="1" t="s">
+      <c r="EJ1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="EJ1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="EK1" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="EL1" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="EM1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="EN1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="EO1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="EP1" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="EQ1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="ES1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="ER1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="ES1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="ET1" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="EU1" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="EV1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="EW1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="EX1" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="EY1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="FA1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="EZ1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="FA1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="FB1" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="FC1" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="FD1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="FG1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="FH1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="FI1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="FH1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="FI1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="FK1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="FJ1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="FK1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="FL1" s="1" t="s">
         <v>15</v>
@@ -1685,610 +1682,610 @@
         <v>12</v>
       </c>
       <c r="FN1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="FQ1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="FT1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="FU1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="FV1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="FW1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="FX1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="FY1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="FZ1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="GA1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="GB1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="GC1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="GA1" s="1" t="s">
+      <c r="GD1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="GB1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="GC1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="GD1" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="GE1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="GF1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="GG1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="GH1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="GI1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="GJ1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="GK1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="GG1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="GH1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="GI1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="GJ1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="GK1" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="GL1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="GM1" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="GN1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="GO1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="GP1" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="GQ1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="GR1" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="GS1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="GT1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="GU1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="GV1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="GW1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="GX1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="GT1" s="1" t="s">
+      <c r="GY1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="GU1" s="1" t="s">
+      <c r="GZ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="HA1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="GV1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="GW1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="GX1" s="1" t="s">
+      <c r="HB1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="GY1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="GZ1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="HA1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="HB1" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="HC1" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="HD1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="HE1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="HF1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="HG1" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="HH1" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="HI1" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="HJ1" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="HK1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="HL1" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="HM1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="HN1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="HO1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="HP1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="HO1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="HP1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="HQ1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="HR1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="HS1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="HT1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="HU1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="HV1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="HW1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="HX1" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="HY1" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="HZ1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="IA1" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="IB1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="IC1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="ID1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="ID1" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="IE1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="IF1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="IG1" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="IH1" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="II1" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="IJ1" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="IK1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="IL1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="IM1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="IN1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="IO1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="IP1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="IQ1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="IR1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="IS1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="IT1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="IU1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="IV1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="IN1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="IO1" s="1" t="s">
+      <c r="IW1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="IP1" s="1" t="s">
+      <c r="IX1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="IY1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="IZ1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="JA1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="JB1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="IQ1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="IR1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="IS1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="IT1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="IU1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="IV1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="IW1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="IX1" s="1" t="s">
+      <c r="JC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="JD1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="JE1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="JF1" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="IY1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="IZ1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="JA1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="JB1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="JC1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="JD1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="JE1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="JF1" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="JG1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="JH1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="JI1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="JJ1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="JK1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="JL1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="JM1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="JN1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="JI1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="JJ1" s="1" t="s">
+      <c r="JO1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="JP1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="JQ1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="JR1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="JK1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="JL1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="JM1" s="1" t="s">
+      <c r="JS1" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="JN1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="JO1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="JP1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="JQ1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="JR1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="JS1" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="JT1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="JU1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="JV1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="JW1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="JX1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="JY1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="JZ1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="KA1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="KB1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="KC1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="KD1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="KD1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="KE1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="KF1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="KG1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="KH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="KI1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="KJ1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="KK1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="KL1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="KM1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="KF1" s="1" t="s">
+      <c r="KN1" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="KG1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="KH1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="KI1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="KJ1" s="1" t="s">
+      <c r="KO1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="KP1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="KK1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="KL1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KM1" s="1" t="s">
+      <c r="KQ1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="KN1" s="1" t="s">
+      <c r="KR1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="KO1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="KP1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="KQ1" s="1" t="s">
+      <c r="KS1" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="KR1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="KS1" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="KT1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="KU1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="KV1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="KW1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="KX1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="KY1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="KV1" s="1" t="s">
+      <c r="KZ1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="KW1" s="1" t="s">
+      <c r="LA1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="KX1" s="1" t="s">
+      <c r="LB1" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="KY1" s="1" t="s">
+      <c r="LC1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="LD1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="KZ1" s="1" t="s">
+      <c r="LE1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="LA1" s="1" t="s">
+      <c r="LF1" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="LB1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="LC1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="LD1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="LE1" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="LF1" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="LG1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="LH1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="LI1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="LJ1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="LK1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="LL1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="LM1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="LN1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="LO1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="LK1" s="1" t="s">
+      <c r="LP1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="LQ1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="LL1" s="1" t="s">
+      <c r="LR1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="LS1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="LT1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="LM1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="LN1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="LO1" s="1" t="s">
+      <c r="LU1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="LV1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="LW1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="LX1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="LP1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="LQ1" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="LR1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="LS1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="LT1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="LU1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="LV1" s="1" t="s">
+      <c r="LY1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="LW1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="LX1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="LY1" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="LZ1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="MA1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="MB1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="MC1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="MD1" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="ME1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="MF1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="MG1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="MH1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="MF1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="MG1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="MH1" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="MI1" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="MJ1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="MK1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="ML1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="MM1" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="MN1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="MO1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="MP1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="MQ1" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="MR1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="MS1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="MT1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="MU1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="MV1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="MW1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="MU1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="MV1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="MW1" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="MX1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="MY1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="MZ1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="NA1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="NB1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:366" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:366" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:366" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>